<commit_message>
Auto‑update: 2025-05-21 01:12:13 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B157"/>
+  <dimension ref="A1:C157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>word</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>severity</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -454,6 +459,9 @@
           <t>Ahmoq</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -464,6 +472,9 @@
           <t>Am</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -474,6 +485,9 @@
           <t>Befarosat</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -484,6 +498,9 @@
           <t>Cho'choq</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -494,6 +511,9 @@
           <t>Dalban</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -504,6 +524,9 @@
           <t>Dalbayob</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -514,6 +537,9 @@
           <t>Dalbayop</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -524,6 +550,9 @@
           <t>Dnx</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -534,6 +563,9 @@
           <t>Dovdir</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -544,6 +576,9 @@
           <t>Foxisha</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -554,6 +589,9 @@
           <t>Fuck</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -564,6 +602,9 @@
           <t>Fuck you</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -574,6 +615,9 @@
           <t>Gandon</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -584,6 +628,9 @@
           <t>Haromi</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -594,6 +641,9 @@
           <t>Hunasa</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -604,6 +654,9 @@
           <t>Iflos</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -614,6 +667,9 @@
           <t>Iplos</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -624,6 +680,9 @@
           <t>Isqirt</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -633,6 +692,9 @@
         <is>
           <t>Jalab</t>
         </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -644,6 +706,9 @@
           <t>Jalla</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -654,6 +719,9 @@
           <t>Jallap</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -664,6 +732,9 @@
           <t>Jinni</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -674,6 +745,9 @@
           <t>Jipiriq</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -684,6 +758,9 @@
           <t>Kot</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -694,6 +771,9 @@
           <t>Kotinga</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -704,6 +784,9 @@
           <t>Koʻt</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -714,6 +797,9 @@
           <t>Lox</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -724,6 +810,9 @@
           <t>Manjalaqi</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -734,6 +823,9 @@
           <t>Maraz</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -744,6 +836,9 @@
           <t>Mol miyya</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -754,6 +849,9 @@
           <t>Om</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -764,6 +862,9 @@
           <t>Pidaraz</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -774,6 +875,9 @@
           <t>Pidr</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -784,6 +888,9 @@
           <t>Pipez</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -794,6 +901,9 @@
           <t>Pizdes</t>
         </is>
       </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -804,6 +914,9 @@
           <t>Poxuy</t>
         </is>
       </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -814,6 +927,9 @@
           <t>Poxxuy</t>
         </is>
       </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -824,6 +940,9 @@
           <t>Pzds</t>
         </is>
       </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -834,6 +953,9 @@
           <t>Pzdss</t>
         </is>
       </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -844,6 +966,9 @@
           <t>Qanchiq</t>
         </is>
       </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -854,6 +979,9 @@
           <t>Qanciq</t>
         </is>
       </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -864,6 +992,9 @@
           <t>Qanjiq</t>
         </is>
       </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -874,6 +1005,9 @@
           <t>Qetoq</t>
         </is>
       </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -884,6 +1018,9 @@
           <t>Qotaqxor</t>
         </is>
       </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -894,6 +1031,9 @@
           <t>Qoto</t>
         </is>
       </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -904,6 +1044,9 @@
           <t>Qotoq</t>
         </is>
       </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -914,6 +1057,9 @@
           <t>Qotoqbosh</t>
         </is>
       </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -924,6 +1070,9 @@
           <t>Qo’toq</t>
         </is>
       </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -934,6 +1083,9 @@
           <t>Sen qishloqlisan</t>
         </is>
       </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -944,6 +1096,9 @@
           <t>Sik</t>
         </is>
       </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -954,6 +1109,9 @@
           <t>Sikaman</t>
         </is>
       </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -964,6 +1122,9 @@
           <t>Sikdim</t>
         </is>
       </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -974,6 +1135,9 @@
           <t>Ske</t>
         </is>
       </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -984,6 +1148,9 @@
           <t>Suchka</t>
         </is>
       </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -994,6 +1161,9 @@
           <t>Suka</t>
         </is>
       </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1004,6 +1174,9 @@
           <t>Tashoq</t>
         </is>
       </c>
+      <c r="C57" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1014,6 +1187,9 @@
           <t>Tashshoq</t>
         </is>
       </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1024,6 +1200,9 @@
           <t>Tashshoq sho’rva</t>
         </is>
       </c>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1034,6 +1213,9 @@
           <t>Tente</t>
         </is>
       </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1044,6 +1226,9 @@
           <t>Xaromi</t>
         </is>
       </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1054,6 +1239,9 @@
           <t>Ya yebal tebya</t>
         </is>
       </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1064,6 +1252,9 @@
           <t>Yban</t>
         </is>
       </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1074,6 +1265,9 @@
           <t>Ybat</t>
         </is>
       </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1084,6 +1278,9 @@
           <t>Yeban</t>
         </is>
       </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1094,6 +1291,9 @@
           <t>Yebanutiy</t>
         </is>
       </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1104,6 +1304,9 @@
           <t>Yiban</t>
         </is>
       </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1114,6 +1317,9 @@
           <t>Zaybal</t>
         </is>
       </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1124,6 +1330,9 @@
           <t>ahmoq</t>
         </is>
       </c>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1134,6 +1343,9 @@
           <t>ahuel</t>
         </is>
       </c>
+      <c r="C70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1144,6 +1356,9 @@
           <t>am</t>
         </is>
       </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1154,6 +1369,9 @@
           <t>amcha</t>
         </is>
       </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1164,6 +1382,9 @@
           <t>aminga</t>
         </is>
       </c>
+      <c r="C73" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1174,6 +1395,9 @@
           <t>basharenga qotogm</t>
         </is>
       </c>
+      <c r="C74" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1184,6 +1408,9 @@
           <t>bitch</t>
         </is>
       </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1194,6 +1421,9 @@
           <t>ble</t>
         </is>
       </c>
+      <c r="C76" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1204,6 +1434,9 @@
           <t>blet</t>
         </is>
       </c>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1214,6 +1447,9 @@
           <t>bo'qidish</t>
         </is>
       </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1224,6 +1460,9 @@
           <t>bo'qkalla</t>
         </is>
       </c>
+      <c r="C79" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1234,6 +1473,9 @@
           <t>boq</t>
         </is>
       </c>
+      <c r="C80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1244,6 +1486,9 @@
           <t>chmo</t>
         </is>
       </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1254,6 +1499,9 @@
           <t>chumo</t>
         </is>
       </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -1264,6 +1512,9 @@
           <t>dabba</t>
         </is>
       </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1274,6 +1525,9 @@
           <t>dalbayob</t>
         </is>
       </c>
+      <c r="C84" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1284,6 +1538,9 @@
           <t>daun</t>
         </is>
       </c>
+      <c r="C85" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -1294,6 +1551,9 @@
           <t>dinnaxuy</t>
         </is>
       </c>
+      <c r="C86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1304,6 +1564,9 @@
           <t>fuck</t>
         </is>
       </c>
+      <c r="C87" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1314,6 +1577,9 @@
           <t>fucking</t>
         </is>
       </c>
+      <c r="C88" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1324,6 +1590,9 @@
           <t>gandon</t>
         </is>
       </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1334,6 +1603,9 @@
           <t>gay</t>
         </is>
       </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -1344,6 +1616,9 @@
           <t>gey</t>
         </is>
       </c>
+      <c r="C91" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -1354,6 +1629,9 @@
           <t>gnida</t>
         </is>
       </c>
+      <c r="C92" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -1364,6 +1642,9 @@
           <t>haromi</t>
         </is>
       </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -1374,6 +1655,9 @@
           <t>hunasa</t>
         </is>
       </c>
+      <c r="C94" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -1384,6 +1668,9 @@
           <t>itbet</t>
         </is>
       </c>
+      <c r="C95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -1394,6 +1681,9 @@
           <t>jala</t>
         </is>
       </c>
+      <c r="C96" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -1404,6 +1694,9 @@
           <t>jala ble</t>
         </is>
       </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -1414,6 +1707,9 @@
           <t>jalaaap</t>
         </is>
       </c>
+      <c r="C98" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -1424,6 +1720,9 @@
           <t>jalab</t>
         </is>
       </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -1434,6 +1733,9 @@
           <t>jalap</t>
         </is>
       </c>
+      <c r="C100" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -1444,6 +1746,9 @@
           <t>jalla</t>
         </is>
       </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -1454,6 +1759,9 @@
           <t>jallap</t>
         </is>
       </c>
+      <c r="C102" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -1464,6 +1772,9 @@
           <t>ko't</t>
         </is>
       </c>
+      <c r="C103" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -1474,6 +1785,9 @@
           <t>kot</t>
         </is>
       </c>
+      <c r="C104" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -1484,6 +1798,9 @@
           <t>nedagon</t>
         </is>
       </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -1494,6 +1811,9 @@
           <t>nigga</t>
         </is>
       </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -1504,6 +1824,9 @@
           <t>nigger</t>
         </is>
       </c>
+      <c r="C107" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -1514,6 +1837,9 @@
           <t>om</t>
         </is>
       </c>
+      <c r="C108" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -1524,6 +1850,9 @@
           <t>onangni</t>
         </is>
       </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -1534,6 +1863,9 @@
           <t>oom</t>
         </is>
       </c>
+      <c r="C110" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -1544,6 +1876,9 @@
           <t>p1zdes</t>
         </is>
       </c>
+      <c r="C111" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -1554,6 +1889,9 @@
           <t>pidaras</t>
         </is>
       </c>
+      <c r="C112" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -1564,6 +1902,9 @@
           <t>pidaraz</t>
         </is>
       </c>
+      <c r="C113" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -1574,6 +1915,9 @@
           <t>pidr</t>
         </is>
       </c>
+      <c r="C114" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -1584,6 +1928,9 @@
           <t>pizda</t>
         </is>
       </c>
+      <c r="C115" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -1594,6 +1941,9 @@
           <t>pizdes</t>
         </is>
       </c>
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -1604,6 +1954,9 @@
           <t>qanjiq</t>
         </is>
       </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -1614,6 +1967,9 @@
           <t>qo'toq</t>
         </is>
       </c>
+      <c r="C118" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -1624,6 +1980,9 @@
           <t>qo'toqbosh</t>
         </is>
       </c>
+      <c r="C119" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -1634,6 +1993,9 @@
           <t>qotaq</t>
         </is>
       </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -1644,6 +2006,9 @@
           <t>qoto</t>
         </is>
       </c>
+      <c r="C121" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -1654,6 +2019,9 @@
           <t>qotoq</t>
         </is>
       </c>
+      <c r="C122" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -1664,6 +2032,9 @@
           <t>qutoq</t>
         </is>
       </c>
+      <c r="C123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -1674,6 +2045,9 @@
           <t>seks</t>
         </is>
       </c>
+      <c r="C124" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -1684,6 +2058,9 @@
           <t>seksi baby</t>
         </is>
       </c>
+      <c r="C125" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -1694,6 +2071,9 @@
           <t>sex</t>
         </is>
       </c>
+      <c r="C126" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -1704,6 +2084,9 @@
           <t>sikay</t>
         </is>
       </c>
+      <c r="C127" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -1714,6 +2097,9 @@
           <t>sike</t>
         </is>
       </c>
+      <c r="C128" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -1724,6 +2110,9 @@
           <t>sikish</t>
         </is>
       </c>
+      <c r="C129" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -1734,6 +2123,9 @@
           <t>siktim</t>
         </is>
       </c>
+      <c r="C130" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -1744,6 +2136,9 @@
           <t>sikvoti</t>
         </is>
       </c>
+      <c r="C131" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -1754,6 +2149,9 @@
           <t>skay</t>
         </is>
       </c>
+      <c r="C132" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -1764,6 +2162,9 @@
           <t>ske</t>
         </is>
       </c>
+      <c r="C133" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -1774,6 +2175,9 @@
           <t>skey</t>
         </is>
       </c>
+      <c r="C134" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -1784,6 +2188,9 @@
           <t>suchka</t>
         </is>
       </c>
+      <c r="C135" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -1794,6 +2201,9 @@
           <t>suka</t>
         </is>
       </c>
+      <c r="C136" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -1804,6 +2214,9 @@
           <t>sukka</t>
         </is>
       </c>
+      <c r="C137" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -1814,6 +2227,9 @@
           <t>tashsho</t>
         </is>
       </c>
+      <c r="C138" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -1824,6 +2240,9 @@
           <t>tupoy</t>
         </is>
       </c>
+      <c r="C139" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -1834,6 +2253,9 @@
           <t>tvar</t>
         </is>
       </c>
+      <c r="C140" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -1844,6 +2266,9 @@
           <t>tvariddin</t>
         </is>
       </c>
+      <c r="C141" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -1854,6 +2279,9 @@
           <t>wtf</t>
         </is>
       </c>
+      <c r="C142" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -1864,6 +2292,9 @@
           <t>xaromi</t>
         </is>
       </c>
+      <c r="C143" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -1874,6 +2305,9 @@
           <t>xuyeplet</t>
         </is>
       </c>
+      <c r="C144" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -1884,6 +2318,9 @@
           <t>xuyesos</t>
         </is>
       </c>
+      <c r="C145" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -1894,6 +2331,9 @@
           <t>xuyila</t>
         </is>
       </c>
+      <c r="C146" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -1904,6 +2344,9 @@
           <t>yban</t>
         </is>
       </c>
+      <c r="C147" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -1914,6 +2357,9 @@
           <t>yeban</t>
         </is>
       </c>
+      <c r="C148" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -1924,6 +2370,9 @@
           <t>yebanashka</t>
         </is>
       </c>
+      <c r="C149" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -1934,6 +2383,9 @@
           <t>yebat</t>
         </is>
       </c>
+      <c r="C150" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -1944,6 +2396,9 @@
           <t>yebbat</t>
         </is>
       </c>
+      <c r="C151" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -1954,6 +2409,9 @@
           <t>yebnu</t>
         </is>
       </c>
+      <c r="C152" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -1964,6 +2422,9 @@
           <t>yebu</t>
         </is>
       </c>
+      <c r="C153" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -1974,6 +2435,9 @@
           <t>yetim</t>
         </is>
       </c>
+      <c r="C154" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -1984,6 +2448,9 @@
           <t>yetm</t>
         </is>
       </c>
+      <c r="C155" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -1994,6 +2461,9 @@
           <t>yiban</t>
         </is>
       </c>
+      <c r="C156" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -2003,6 +2473,9 @@
         <is>
           <t>yibanat</t>
         </is>
+      </c>
+      <c r="C157" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto‑update: 2025-05-30 19:19:27 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,146 +473,146 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>208</v>
+        <v>321</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Befarosat</t>
+          <t>Amcha</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>170</v>
+        <v>208</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cho'choq</t>
+          <t>Befarosat</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>196</v>
+        <v>319</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dalban</t>
+          <t>Blyat</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>170</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dalbayob</t>
+          <t>Cho'choq</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dalbayop</t>
+          <t>Dalban</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dnx</t>
+          <t>Dalbayob</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6</v>
+        <v>238</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dovdir</t>
+          <t>Dalbayop</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>272</v>
+        <v>127</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Foxisha</t>
+          <t>Dnx</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fuck</t>
+          <t>Dovdir</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>152</v>
+        <v>320</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Fuck you</t>
+          <t>Ey qetoq</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>209</v>
+        <v>272</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Gandon</t>
+          <t>Foxisha</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -621,11 +621,11 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Haromi</t>
+          <t>Fuck</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -634,11 +634,11 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>197</v>
+        <v>152</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Hunasa</t>
+          <t>Fuck you</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -647,11 +647,11 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Iflos</t>
+          <t>Gandon</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -660,11 +660,11 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>192</v>
+        <v>296</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Iplos</t>
+          <t>Gotalak</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -673,11 +673,11 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Isqirt</t>
+          <t>Haromi</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -686,11 +686,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>197</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jalab</t>
+          <t>Hunasa</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -699,11 +699,11 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jalla</t>
+          <t>Iflos</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -712,11 +712,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>151</v>
+        <v>192</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jallap</t>
+          <t>Iplos</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -725,11 +725,11 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Jinni</t>
+          <t>Isqirt</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -738,11 +738,11 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>205</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jipiriq</t>
+          <t>Jalab</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -751,11 +751,11 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>195</v>
+        <v>214</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Kot</t>
+          <t>Jalla</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -764,11 +764,11 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>65</v>
+        <v>151</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Kotinga</t>
+          <t>Jallap</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -777,11 +777,11 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>194</v>
+        <v>56</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Koʻt</t>
+          <t>Jinni</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -790,11 +790,11 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lox</t>
+          <t>Jipiriq</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -803,24 +803,24 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>190</v>
+        <v>323</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Manjalaqi</t>
+          <t>Kispurush</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>271</v>
+        <v>195</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Maraz</t>
+          <t>Kot</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -829,11 +829,11 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>207</v>
+        <v>65</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Mol miyya</t>
+          <t>Kotinga</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -842,11 +842,11 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Om</t>
+          <t>Koʻt</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -855,11 +855,11 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>5</v>
+        <v>129</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Pidaraz</t>
+          <t>Lox</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -868,11 +868,11 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>295</v>
+        <v>190</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Pidr</t>
+          <t>Manjalaqi</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -881,11 +881,11 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>156</v>
+        <v>271</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Pipez</t>
+          <t>Maraz</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -894,11 +894,11 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Pizdes</t>
+          <t>Mol miyya</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -907,11 +907,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>115</v>
+        <v>212</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Poxuy</t>
+          <t>Om</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -920,37 +920,37 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>114</v>
+        <v>318</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Poxxuy</t>
+          <t>Onangni sikay</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>154</v>
+        <v>317</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Pzds</t>
+          <t>Onenei ami</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>155</v>
+        <v>298</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Pzdss</t>
+          <t>Pasholak</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -959,11 +959,11 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>269</v>
+        <v>5</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Qanchiq</t>
+          <t>Pidaraz</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -972,11 +972,11 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>270</v>
+        <v>295</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Qanciq</t>
+          <t>Pidr</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -985,11 +985,11 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Qanjiq</t>
+          <t>Pipez</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -998,11 +998,11 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Qetoq</t>
+          <t>Pizdes</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1011,11 +1011,11 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>172</v>
+        <v>115</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Qotaqxor</t>
+          <t>Poxuy</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1024,11 +1024,11 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>257</v>
+        <v>114</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Qoto</t>
+          <t>Poxxuy</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1037,11 +1037,11 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Qotoq</t>
+          <t>Pzds</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1050,11 +1050,11 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Qotoqbosh</t>
+          <t>Pzdss</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1063,11 +1063,11 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>210</v>
+        <v>269</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Qo’toq</t>
+          <t>Qanchiq</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1076,11 +1076,11 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Sen qishloqlisan</t>
+          <t>Qanciq</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1089,11 +1089,11 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Sik</t>
+          <t>Qanjiq</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1102,11 +1102,11 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Sikaman</t>
+          <t>Qetoq</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1115,11 +1115,11 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Sikdim</t>
+          <t>Qotaqxor</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1128,11 +1128,11 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>153</v>
+        <v>257</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ske</t>
+          <t>Qoto</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1141,11 +1141,11 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>297</v>
+        <v>169</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Suchka</t>
+          <t>Qotoq</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1154,11 +1154,11 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Suka</t>
+          <t>Qotoqbosh</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1167,11 +1167,11 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Tashoq</t>
+          <t>Qo’toq</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1180,11 +1180,11 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>217</v>
+        <v>302</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Tashshoq</t>
+          <t>Sen qishloqlisan</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1193,11 +1193,11 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Tashshoq sho’rva</t>
+          <t>Sik</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1206,11 +1206,11 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Tente</t>
+          <t>Sikaman</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1219,11 +1219,11 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Xaromi</t>
+          <t>Sikdim</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1232,11 +1232,11 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ya yebal tebya</t>
+          <t>Ske</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1245,11 +1245,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>233</v>
+        <v>297</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Yban</t>
+          <t>Suchka</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1258,11 +1258,11 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>198</v>
+        <v>4</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ybat</t>
+          <t>Suka</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1271,11 +1271,11 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>15</v>
+        <v>218</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Yeban</t>
+          <t>Tashoq</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1284,11 +1284,11 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Yebanutiy</t>
+          <t>Tashshoq</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1297,24 +1297,24 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2</v>
+        <v>316</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Yiban</t>
+          <t>Tashshoq sho'rva</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>183</v>
+        <v>219</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Zaybal</t>
+          <t>Tashshoq sho’rva</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1323,11 +1323,11 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ahmoq</t>
+          <t>Tente</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1336,11 +1336,11 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ahuel</t>
+          <t>Xaromi</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1349,11 +1349,11 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>22</v>
+        <v>143</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>am</t>
+          <t>Ya yebal tebya</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1362,11 +1362,11 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>amcha</t>
+          <t>Yban</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1375,11 +1375,11 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>108</v>
+        <v>198</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>aminga</t>
+          <t>Ybat</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1388,11 +1388,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>236</v>
+        <v>15</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>basharenga qotogm</t>
+          <t>Yeban</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1401,11 +1401,11 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>Yebanutiy</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1414,11 +1414,11 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>Yiban</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1427,11 +1427,11 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>Zaybal</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1440,11 +1440,11 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>261</v>
+        <v>78</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>ahmoq</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1453,11 +1453,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>262</v>
+        <v>142</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>ahuel</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1466,11 +1466,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>244</v>
+        <v>22</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>am</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1479,11 +1479,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>279</v>
+        <v>223</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>amcha</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1492,11 +1492,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>280</v>
+        <v>108</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>aminga</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1505,11 +1505,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>305</v>
+        <v>236</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>basharenga qotogm</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1518,11 +1518,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>278</v>
+        <v>99</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1544,11 +1544,11 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1557,11 +1557,11 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>110</v>
+        <v>261</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>111</v>
+        <v>262</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1583,11 +1583,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>160</v>
+        <v>244</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1596,11 +1596,11 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>167</v>
+        <v>279</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1609,11 +1609,11 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>166</v>
+        <v>280</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,11 +1622,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>161</v>
+        <v>305</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1635,11 +1635,11 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>227</v>
+        <v>107</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1648,11 +1648,11 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>203</v>
+        <v>278</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1661,11 +1661,11 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>260</v>
+        <v>84</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1674,11 +1674,11 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1687,11 +1687,11 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1700,11 +1700,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>303</v>
+        <v>160</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,11 +1713,11 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>76</v>
+        <v>167</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1726,11 +1726,11 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1739,11 +1739,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>88</v>
+        <v>161</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>89</v>
+        <v>227</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>33</v>
+        <v>203</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,11 +1778,11 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1791,11 +1791,11 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>306</v>
+        <v>95</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>199</v>
+        <v>98</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>83</v>
+        <v>303</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,11 +1830,11 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,11 +1843,11 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1856,11 +1856,11 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>184</v>
+        <v>88</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1869,11 +1869,11 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,11 +1882,11 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1895,11 +1895,11 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1908,37 +1908,37 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>97</v>
+        <v>310</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>86</v>
+        <v>293</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>11</v>
+        <v>306</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,11 +1947,11 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>92</v>
+        <v>199</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,11 +1960,11 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -1973,11 +1973,11 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1986,11 +1986,11 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -1999,11 +1999,11 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2012,11 +2012,11 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>282</v>
+        <v>75</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,11 +2038,11 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2051,11 +2051,11 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2064,11 +2064,11 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2077,11 +2077,11 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,11 +2129,11 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2142,11 +2142,11 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>73</v>
+        <v>234</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2155,11 +2155,11 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>159</v>
+        <v>282</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2181,11 +2181,11 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2194,11 +2194,11 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>119</v>
+        <v>13</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,24 +2220,24 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>87</v>
+        <v>322</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2246,11 +2246,11 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2259,11 +2259,11 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>163</v>
+        <v>18</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2272,11 +2272,11 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>137</v>
+        <v>20</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2285,11 +2285,11 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2298,11 +2298,11 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>140</v>
+        <v>73</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2311,11 +2311,11 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,11 +2324,11 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2337,11 +2337,11 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2350,11 +2350,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>281</v>
+        <v>90</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>148</v>
+        <v>119</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>287</v>
+        <v>87</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,11 +2389,11 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2402,11 +2402,11 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>277</v>
+        <v>140</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,14 +2467,170 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
+        <v>139</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>xuyesos</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>141</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>xuyila</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>19</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>yban</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>281</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>yeban</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>148</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>yebanashka</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>287</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>yebat</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>91</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>yebbat</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>145</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>yebnu</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>144</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>yebu</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>14</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>94</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>277</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
         <v>283</v>
       </c>
-      <c r="B157" t="inlineStr">
+      <c r="B169" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C157" t="n">
+      <c r="C169" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-06-14 19:18:23 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:C173"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,24 +816,24 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>195</v>
+        <v>326</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Kot</t>
+          <t>Ko't</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kotinga</t>
+          <t>Kot</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -842,11 +842,11 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Koʻt</t>
+          <t>Kotinga</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -855,11 +855,11 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>129</v>
+        <v>194</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Lox</t>
+          <t>Koʻt</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -868,11 +868,11 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>190</v>
+        <v>129</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Manjalaqi</t>
+          <t>Lox</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -881,11 +881,11 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>271</v>
+        <v>190</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Maraz</t>
+          <t>Manjalaqi</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -894,11 +894,11 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>207</v>
+        <v>271</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mol miyya</t>
+          <t>Maraz</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -907,11 +907,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Om</t>
+          <t>Mol miyya</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -920,24 +920,24 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>318</v>
+        <v>212</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Onangni sikay</t>
+          <t>Om</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Onenei ami</t>
+          <t>Onangni sikay</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -946,24 +946,24 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Pasholak</t>
+          <t>Onenei ami</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Pidaraz</t>
+          <t>Pasholak</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -972,11 +972,11 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>295</v>
+        <v>5</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Pidr</t>
+          <t>Pidaraz</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -985,11 +985,11 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>156</v>
+        <v>295</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Pipez</t>
+          <t>Pidr</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -998,11 +998,11 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Pizdes</t>
+          <t>Pipez</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1011,11 +1011,11 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Poxuy</t>
+          <t>Pizdes</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1024,11 +1024,11 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Poxxuy</t>
+          <t>Poxuy</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1037,11 +1037,11 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Pzds</t>
+          <t>Poxxuy</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1050,24 +1050,24 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>155</v>
+        <v>325</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Pzdss</t>
+          <t>Pzdc</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>269</v>
+        <v>154</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Qanchiq</t>
+          <t>Pzds</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1076,11 +1076,11 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>270</v>
+        <v>155</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Qanciq</t>
+          <t>Pzdss</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1089,11 +1089,11 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>189</v>
+        <v>269</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Qanjiq</t>
+          <t>Qanchiq</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1102,11 +1102,11 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>211</v>
+        <v>270</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Qetoq</t>
+          <t>Qanciq</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1115,11 +1115,11 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Qotaqxor</t>
+          <t>Qanjiq</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1128,11 +1128,11 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>257</v>
+        <v>211</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Qoto</t>
+          <t>Qetoq</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1141,11 +1141,11 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Qotoq</t>
+          <t>Qotaqxor</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1154,11 +1154,11 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>25</v>
+        <v>257</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Qotoqbosh</t>
+          <t>Qoto</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1167,11 +1167,11 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>210</v>
+        <v>169</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Qo’toq</t>
+          <t>Qotoq</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1180,11 +1180,11 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>302</v>
+        <v>25</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Sen qishloqlisan</t>
+          <t>Qotoqbosh</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1193,11 +1193,11 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sik</t>
+          <t>Qo’toq</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1206,11 +1206,11 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>215</v>
+        <v>302</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sikaman</t>
+          <t>Sen qishloqlisan</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1219,11 +1219,11 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sikdim</t>
+          <t>Sik</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1232,11 +1232,11 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ske</t>
+          <t>Sikaman</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1245,11 +1245,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>297</v>
+        <v>113</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Suchka</t>
+          <t>Sikdim</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1258,11 +1258,11 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>4</v>
+        <v>153</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Suka</t>
+          <t>Ske</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1271,11 +1271,11 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>218</v>
+        <v>297</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Tashoq</t>
+          <t>Suchka</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1284,11 +1284,11 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>217</v>
+        <v>4</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Tashshoq</t>
+          <t>Suka</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1297,24 +1297,24 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>316</v>
+        <v>218</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Tashshoq sho'rva</t>
+          <t>Tashoq</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Tashshoq sho’rva</t>
+          <t>Tashshoq</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1323,24 +1323,24 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>176</v>
+        <v>316</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Tente</t>
+          <t>Tashshoq sho'rva</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>64</v>
+        <v>219</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Xaromi</t>
+          <t>Tashshoq sho’rva</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1349,11 +1349,11 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ya yebal tebya</t>
+          <t>Tente</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1362,11 +1362,11 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>233</v>
+        <v>64</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Yban</t>
+          <t>Xaromi</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1375,11 +1375,11 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>198</v>
+        <v>143</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Ybat</t>
+          <t>Ya yebal tebya</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1388,11 +1388,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Yeban</t>
+          <t>Yban</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1401,11 +1401,11 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Yebanutiy</t>
+          <t>Ybat</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1414,11 +1414,11 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Yiban</t>
+          <t>Yeban</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1427,11 +1427,11 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Zaybal</t>
+          <t>Yebanutiy</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1440,11 +1440,11 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>ahmoq</t>
+          <t>Yiban</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1453,11 +1453,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>ahuel</t>
+          <t>Zaybal</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1466,11 +1466,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>am</t>
+          <t>ahmoq</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1479,11 +1479,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>223</v>
+        <v>142</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>amcha</t>
+          <t>ahuel</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1492,11 +1492,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>aminga</t>
+          <t>am</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1505,11 +1505,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>basharenga qotogm</t>
+          <t>amcha</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1518,11 +1518,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>aminga</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>99</v>
+        <v>236</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>basharenga qotogm</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1544,11 +1544,11 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1557,11 +1557,11 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>261</v>
+        <v>99</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>262</v>
+        <v>53</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1583,11 +1583,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1596,11 +1596,11 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1609,11 +1609,11 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,11 +1622,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1635,11 +1635,11 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>107</v>
+        <v>280</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1648,11 +1648,11 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1661,11 +1661,11 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1674,11 +1674,11 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1687,11 +1687,11 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1700,11 +1700,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,24 +1713,24 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>167</v>
+        <v>324</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1739,11 +1739,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>227</v>
+        <v>167</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,11 +1778,11 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>260</v>
+        <v>161</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1791,11 +1791,11 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>95</v>
+        <v>227</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>98</v>
+        <v>203</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,11 +1830,11 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,11 +1843,11 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1856,11 +1856,11 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>88</v>
+        <v>303</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1869,11 +1869,11 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,11 +1882,11 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1895,11 +1895,11 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1908,37 +1908,37 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>310</v>
+        <v>89</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>293</v>
+        <v>33</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>306</v>
+        <v>26</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,37 +1947,37 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>199</v>
+        <v>310</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>83</v>
+        <v>293</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>23</v>
+        <v>306</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1986,11 +1986,11 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>96</v>
+        <v>199</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -1999,11 +1999,11 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2012,11 +2012,11 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,24 +2038,24 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>74</v>
+        <v>327</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2064,11 +2064,11 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2077,11 +2077,11 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,11 +2129,11 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2142,11 +2142,11 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>234</v>
+        <v>92</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2155,11 +2155,11 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>282</v>
+        <v>28</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2181,11 +2181,11 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2194,11 +2194,11 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>71</v>
+        <v>234</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,24 +2220,24 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>322</v>
+        <v>282</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2246,11 +2246,11 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2259,11 +2259,11 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2272,24 +2272,24 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>20</v>
+        <v>322</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2298,11 +2298,11 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2311,11 +2311,11 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,11 +2324,11 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2337,11 +2337,11 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2350,11 +2350,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>119</v>
+        <v>21</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,11 +2389,11 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2402,11 +2402,11 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,11 +2493,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2506,11 +2506,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>281</v>
+        <v>140</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2519,11 +2519,11 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,11 +2532,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2545,11 +2545,11 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2558,11 +2558,11 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>145</v>
+        <v>281</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2571,11 +2571,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yebat</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yebbat</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,11 +2610,11 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>277</v>
+        <v>145</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yebnu</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2623,14 +2623,66 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
+        <v>144</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>yebu</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>14</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>94</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>277</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
         <v>283</v>
       </c>
-      <c r="B169" t="inlineStr">
+      <c r="B173" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C169" t="n">
+      <c r="C173" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-07-07 19:21:36 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:C175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1544,24 +1544,24 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>93</v>
+        <v>330</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>bich</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1583,11 +1583,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>261</v>
+        <v>53</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1596,11 +1596,11 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1609,11 +1609,11 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,11 +1622,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1635,11 +1635,11 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1648,11 +1648,11 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1661,11 +1661,11 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>107</v>
+        <v>305</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1674,11 +1674,11 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>278</v>
+        <v>107</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1687,11 +1687,11 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>84</v>
+        <v>278</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1700,11 +1700,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,37 +1713,37 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>324</v>
+        <v>110</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>111</v>
+        <v>324</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,11 +1778,11 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1791,11 +1791,11 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,24 +1830,24 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>95</v>
+        <v>331</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>98</v>
+        <v>260</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1856,11 +1856,11 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>303</v>
+        <v>95</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1869,11 +1869,11 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,11 +1882,11 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>158</v>
+        <v>303</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1895,11 +1895,11 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1908,11 +1908,11 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1921,11 +1921,11 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1934,11 +1934,11 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,63 +1947,63 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>310</v>
+        <v>33</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>199</v>
+        <v>293</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>83</v>
+        <v>306</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2012,11 +2012,11 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>23</v>
+        <v>199</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,24 +2038,24 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>327</v>
+        <v>23</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>184</v>
+        <v>96</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2064,24 +2064,24 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>12</v>
+        <v>327</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>75</v>
+        <v>184</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,11 +2129,11 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2142,11 +2142,11 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2155,11 +2155,11 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2181,11 +2181,11 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2194,11 +2194,11 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>234</v>
+        <v>28</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,11 +2220,11 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>282</v>
+        <v>234</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2233,11 +2233,11 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2246,11 +2246,11 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>71</v>
+        <v>282</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2259,11 +2259,11 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2272,24 +2272,24 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>322</v>
+        <v>71</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2298,24 +2298,24 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>134</v>
+        <v>322</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,11 +2324,11 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2337,11 +2337,11 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2350,11 +2350,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>159</v>
+        <v>73</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,11 +2389,11 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2402,11 +2402,11 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>163</v>
+        <v>32</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,11 +2493,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>27</v>
+        <v>163</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2506,11 +2506,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2519,11 +2519,11 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>139</v>
+        <v>27</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,11 +2532,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2545,11 +2545,11 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>19</v>
+        <v>139</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2558,11 +2558,11 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>281</v>
+        <v>141</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2571,11 +2571,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>148</v>
+        <v>19</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>91</v>
+        <v>148</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,11 +2610,11 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>145</v>
+        <v>287</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>yebat</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2623,11 +2623,11 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>yebbat</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2636,11 +2636,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>14</v>
+        <v>145</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yebnu</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,11 +2649,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yebu</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>277</v>
+        <v>14</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yetim</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2675,14 +2675,40 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
+        <v>94</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>277</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
         <v>283</v>
       </c>
-      <c r="B173" t="inlineStr">
+      <c r="B175" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C173" t="n">
+      <c r="C175" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-09-03 19:19:08 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C175"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,115 +517,115 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cho'choq</t>
+          <t>Buvini ami</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>45</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>196</v>
+        <v>170</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dalban</t>
+          <t>Cho'choq</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>70</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Dalbayob</t>
+          <t>Dalban</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>238</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dalbayop</t>
+          <t>Dalbayob</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>127</v>
+        <v>238</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Dnx</t>
+          <t>Dalbayop</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6</v>
+        <v>127</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Dovdir</t>
+          <t>Dnx</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>320</v>
+        <v>6</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ey qetoq</t>
+          <t>Dovdir</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>95</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>272</v>
+        <v>320</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Foxisha</t>
+          <t>Ey qetoq</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>63</v>
+        <v>272</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fuck</t>
+          <t>Foxisha</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -634,11 +634,11 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fuck you</t>
+          <t>Fuck</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -647,11 +647,11 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>209</v>
+        <v>152</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gandon</t>
+          <t>Fuck you</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -660,11 +660,11 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>296</v>
+        <v>209</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Gotalak</t>
+          <t>Gandon</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -673,11 +673,11 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>29</v>
+        <v>296</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Haromi</t>
+          <t>Gotalak</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -686,11 +686,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>197</v>
+        <v>29</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hunasa</t>
+          <t>Haromi</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -699,11 +699,11 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Iflos</t>
+          <t>Hunasa</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -712,11 +712,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Iplos</t>
+          <t>Iflos</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -725,11 +725,11 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>39</v>
+        <v>192</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Isqirt</t>
+          <t>Iplos</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -738,11 +738,11 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jalab</t>
+          <t>Isqirt</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -751,11 +751,11 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>214</v>
+        <v>1</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Jalla</t>
+          <t>Jalab</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -764,11 +764,11 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Jallap</t>
+          <t>Jalla</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -777,24 +777,24 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>56</v>
+        <v>345</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jinni</t>
+          <t>Jallab</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>205</v>
+        <v>151</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jipiriq</t>
+          <t>Jallap</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -803,63 +803,63 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>323</v>
+        <v>56</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Kispurush</t>
+          <t>Jinni</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>326</v>
+        <v>205</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Ko't</t>
+          <t>Jipiriq</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>195</v>
+        <v>323</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kot</t>
+          <t>Kispurush</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>65</v>
+        <v>326</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Kotinga</t>
+          <t>Ko't</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Koʻt</t>
+          <t>Kot</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -868,11 +868,11 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Lox</t>
+          <t>Kotinga</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -881,11 +881,11 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Manjalaqi</t>
+          <t>Koʻt</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -894,11 +894,11 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>271</v>
+        <v>129</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Maraz</t>
+          <t>Lox</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -907,11 +907,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Mol miyya</t>
+          <t>Manjalaqi</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -920,11 +920,11 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>212</v>
+        <v>271</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Om</t>
+          <t>Maraz</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -933,76 +933,76 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>318</v>
+        <v>207</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Onangni sikay</t>
+          <t>Mol miyya</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>317</v>
+        <v>212</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Onenei ami</t>
+          <t>Om</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Pasholak</t>
+          <t>Onangni sikay</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5</v>
+        <v>317</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Pidaraz</t>
+          <t>Onenei ami</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>295</v>
+        <v>339</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Pidr</t>
+          <t>Opangni omiga ske</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>156</v>
+        <v>298</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Pipez</t>
+          <t>Pasholak</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1011,11 +1011,11 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Pizdes</t>
+          <t>Pidaraz</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1024,11 +1024,11 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>115</v>
+        <v>295</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Poxuy</t>
+          <t>Pidr</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1037,11 +1037,11 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Poxxuy</t>
+          <t>Pipez</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1050,24 +1050,24 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>325</v>
+        <v>213</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Pzdc</t>
+          <t>Pizdes</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Pzds</t>
+          <t>Poxuy</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1076,11 +1076,11 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Pzdss</t>
+          <t>Poxxuy</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1089,24 +1089,24 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>269</v>
+        <v>325</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Qanchiq</t>
+          <t>Pzdc</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>270</v>
+        <v>154</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Qanciq</t>
+          <t>Pzds</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1115,11 +1115,11 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Qanjiq</t>
+          <t>Pzdss</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1128,11 +1128,11 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>211</v>
+        <v>269</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Qetoq</t>
+          <t>Qanchiq</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1141,11 +1141,11 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>172</v>
+        <v>270</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Qotaqxor</t>
+          <t>Qanciq</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1154,11 +1154,11 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>257</v>
+        <v>189</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Qoto</t>
+          <t>Qanjiq</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1167,11 +1167,11 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Qotoq</t>
+          <t>Qetoq</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1180,11 +1180,11 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>25</v>
+        <v>172</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Qotoqbosh</t>
+          <t>Qotaqxor</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1193,11 +1193,11 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>210</v>
+        <v>257</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Qo’toq</t>
+          <t>Qoto</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1206,11 +1206,11 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>302</v>
+        <v>169</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sen qishloqlisan</t>
+          <t>Qotoq</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1219,11 +1219,11 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>216</v>
+        <v>25</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sik</t>
+          <t>Qotoqbosh</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1232,11 +1232,11 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sikaman</t>
+          <t>Qo’toq</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1245,11 +1245,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>113</v>
+        <v>302</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sikdim</t>
+          <t>Sen qishloqlisan</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1258,11 +1258,11 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>153</v>
+        <v>216</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ske</t>
+          <t>Sik</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1271,11 +1271,11 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>297</v>
+        <v>215</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Suchka</t>
+          <t>Sikaman</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1284,11 +1284,11 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Suka</t>
+          <t>Sikdim</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1297,11 +1297,11 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>218</v>
+        <v>153</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Tashoq</t>
+          <t>Ske</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1310,11 +1310,11 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>217</v>
+        <v>297</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Tashshoq</t>
+          <t>Suchka</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1323,24 +1323,24 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>316</v>
+        <v>4</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Tashshoq sho'rva</t>
+          <t>Suka</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Tashshoq sho’rva</t>
+          <t>Tashoq</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1349,11 +1349,11 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>176</v>
+        <v>217</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Tente</t>
+          <t>Tashshoq</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1362,24 +1362,24 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>64</v>
+        <v>316</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Xaromi</t>
+          <t>Tashshoq sho'rva</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Ya yebal tebya</t>
+          <t>Tashshoq sho’rva</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1388,11 +1388,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Yban</t>
+          <t>Tente</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1401,11 +1401,11 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>198</v>
+        <v>64</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Ybat</t>
+          <t>Xaromi</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1414,11 +1414,11 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Yeban</t>
+          <t>Ya yebal tebya</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1427,11 +1427,11 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>62</v>
+        <v>233</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Yebanutiy</t>
+          <t>Yban</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1440,11 +1440,11 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Yiban</t>
+          <t>Ybat</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1453,11 +1453,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>183</v>
+        <v>15</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Zaybal</t>
+          <t>Yeban</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1466,11 +1466,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ahmoq</t>
+          <t>Yebanutiy</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1479,11 +1479,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>142</v>
+        <v>2</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ahuel</t>
+          <t>Yiban</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1492,11 +1492,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>am</t>
+          <t>Zaybal</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1505,11 +1505,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>223</v>
+        <v>78</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>amcha</t>
+          <t>ahmoq</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1518,11 +1518,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>aminga</t>
+          <t>ahuel</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>236</v>
+        <v>22</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>basharenga qotogm</t>
+          <t>am</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1544,24 +1544,24 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>bich</t>
+          <t>ambaliq</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>93</v>
+        <v>223</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>amcha</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>aminga</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1583,11 +1583,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>53</v>
+        <v>236</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>basharenga qotogm</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1596,24 +1596,24 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>261</v>
+        <v>330</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>bich</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>262</v>
+        <v>93</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,11 +1622,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>244</v>
+        <v>99</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1635,11 +1635,11 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>279</v>
+        <v>53</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1648,11 +1648,11 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1661,11 +1661,11 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>305</v>
+        <v>262</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1674,11 +1674,11 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>107</v>
+        <v>244</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1687,11 +1687,11 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1700,11 +1700,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>84</v>
+        <v>280</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,11 +1713,11 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>110</v>
+        <v>305</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1726,24 +1726,24 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>324</v>
+        <v>107</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>111</v>
+        <v>278</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>160</v>
+        <v>84</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,24 +1778,24 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>166</v>
+        <v>324</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>227</v>
+        <v>160</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,24 +1830,24 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>331</v>
+        <v>166</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>260</v>
+        <v>161</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1856,11 +1856,11 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>95</v>
+        <v>227</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1869,11 +1869,11 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>98</v>
+        <v>203</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,37 +1882,37 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>303</v>
+        <v>334</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>idi naxuy</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>76</v>
+        <v>331</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>158</v>
+        <v>260</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1921,11 +1921,11 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1934,11 +1934,11 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,11 +1947,11 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>33</v>
+        <v>303</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,11 +1960,11 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -1973,37 +1973,37 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>310</v>
+        <v>158</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>293</v>
+        <v>88</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>306</v>
+        <v>89</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2012,11 +2012,11 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>199</v>
+        <v>33</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,50 +2038,50 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>23</v>
+        <v>310</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>96</v>
+        <v>293</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,37 +2129,37 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>97</v>
+        <v>327</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>86</v>
+        <v>341</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>onangni sikay</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>11</v>
+        <v>184</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2181,24 +2181,24 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>85</v>
+        <v>333</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>pashol na xuy</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,11 +2220,11 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>234</v>
+        <v>97</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2233,11 +2233,11 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2246,11 +2246,11 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>282</v>
+        <v>11</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2259,11 +2259,11 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2272,11 +2272,11 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2285,11 +2285,11 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2298,24 +2298,24 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>322</v>
+        <v>116</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>109</v>
+        <v>234</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,11 +2324,11 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2337,11 +2337,11 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>18</v>
+        <v>282</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2350,11 +2350,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,24 +2389,24 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>21</v>
+        <v>322</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>162</v>
+        <v>21</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,11 +2493,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2506,11 +2506,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2519,11 +2519,11 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,11 +2532,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2545,11 +2545,11 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2558,11 +2558,11 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2571,11 +2571,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>281</v>
+        <v>163</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,11 +2610,11 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>287</v>
+        <v>27</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2623,11 +2623,11 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2636,11 +2636,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,11 +2649,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2675,11 +2675,11 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>94</v>
+        <v>281</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2688,11 +2688,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>277</v>
+        <v>148</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2701,14 +2701,105 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
+        <v>287</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>yebat</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>91</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>yebbat</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>145</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>yebnu</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>144</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>yebu</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>14</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>94</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>277</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="n">
         <v>283</v>
       </c>
-      <c r="B175" t="inlineStr">
+      <c r="B182" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C175" t="n">
+      <c r="C182" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-10-04 00:45:07 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1180,24 +1180,24 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>172</v>
+        <v>358</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Qotaqxor</t>
+          <t>Qo'taq</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Qoto</t>
+          <t>Qotaqxor</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1206,11 +1206,11 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Qotoq</t>
+          <t>Qoto</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1219,11 +1219,11 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Qotoqbosh</t>
+          <t>Qotoq</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1232,11 +1232,11 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>210</v>
+        <v>25</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Qo’toq</t>
+          <t>Qotoqbosh</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1245,11 +1245,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>302</v>
+        <v>210</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sen qishloqlisan</t>
+          <t>Qo’toq</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1258,24 +1258,24 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>216</v>
+        <v>351</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Sik</t>
+          <t>Seks</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>215</v>
+        <v>302</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Sikaman</t>
+          <t>Sen qishloqlisan</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1284,11 +1284,11 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sikdim</t>
+          <t>Sik</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1297,11 +1297,11 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>153</v>
+        <v>215</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ske</t>
+          <t>Sikaman</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1310,24 +1310,24 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>297</v>
+        <v>352</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Suchka</t>
+          <t>Sikay</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Suka</t>
+          <t>Sikdim</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1336,11 +1336,11 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>218</v>
+        <v>153</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Tashoq</t>
+          <t>Ske</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1349,11 +1349,11 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>217</v>
+        <v>297</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Tashshoq</t>
+          <t>Suchka</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1362,24 +1362,24 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>316</v>
+        <v>4</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Tashshoq sho'rva</t>
+          <t>Suka</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Tashshoq sho’rva</t>
+          <t>Tashoq</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1388,11 +1388,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>176</v>
+        <v>217</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Tente</t>
+          <t>Tashshoq</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1401,24 +1401,24 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>64</v>
+        <v>316</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Xaromi</t>
+          <t>Tashshoq sho'rva</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Ya yebal tebya</t>
+          <t>Tashshoq sho’rva</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1427,11 +1427,11 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>233</v>
+        <v>176</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Yban</t>
+          <t>Tente</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1440,11 +1440,11 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>198</v>
+        <v>64</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Ybat</t>
+          <t>Xaromi</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1453,11 +1453,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Yeban</t>
+          <t>Ya yebal tebya</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1466,11 +1466,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>62</v>
+        <v>233</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Yebanutiy</t>
+          <t>Yban</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1479,11 +1479,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2</v>
+        <v>198</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Yiban</t>
+          <t>Ybat</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1492,11 +1492,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>183</v>
+        <v>15</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Zaybal</t>
+          <t>Yeban</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1505,11 +1505,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>ahmoq</t>
+          <t>Yebanutiy</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1518,11 +1518,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>142</v>
+        <v>2</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ahuel</t>
+          <t>Yiban</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>am</t>
+          <t>Zaybal</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1544,24 +1544,24 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>329</v>
+        <v>78</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ambaliq</t>
+          <t>ahmoq</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>223</v>
+        <v>142</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>amcha</t>
+          <t>ahuel</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>aminga</t>
+          <t>am</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1583,37 +1583,37 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>236</v>
+        <v>329</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>basharenga qotogm</t>
+          <t>ambaliq</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>330</v>
+        <v>223</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>bich</t>
+          <t>amcha</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>aminga</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,37 +1622,37 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>99</v>
+        <v>349</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>amingga ske</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>53</v>
+        <v>360</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>axmoq</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>basharenga qotogm</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1661,24 +1661,24 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>262</v>
+        <v>330</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>bich</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>244</v>
+        <v>93</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1687,11 +1687,11 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>279</v>
+        <v>99</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1700,11 +1700,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>280</v>
+        <v>53</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,11 +1713,11 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>305</v>
+        <v>261</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1726,11 +1726,11 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>107</v>
+        <v>262</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1739,11 +1739,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>84</v>
+        <v>279</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>110</v>
+        <v>280</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,24 +1778,24 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>160</v>
+        <v>278</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,11 +1830,11 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>166</v>
+        <v>110</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,24 +1843,24 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>161</v>
+        <v>324</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>227</v>
+        <v>111</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1869,11 +1869,11 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,37 +1882,37 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>334</v>
+        <v>361</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>idi naxuy</t>
+          <t>garang</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>331</v>
+        <v>167</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>260</v>
+        <v>166</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1921,11 +1921,11 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1934,11 +1934,11 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>98</v>
+        <v>227</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,11 +1947,11 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,50 +1960,50 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>76</v>
+        <v>334</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>idi naxuy</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>158</v>
+        <v>357</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>iflos</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>88</v>
+        <v>331</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>89</v>
+        <v>260</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2012,11 +2012,11 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,37 +2038,37 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>293</v>
+        <v>76</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>306</v>
+        <v>158</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2077,11 +2077,11 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,37 +2129,37 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>onangni sikay</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>184</v>
+        <v>306</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>12</v>
+        <v>199</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2181,24 +2181,24 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>333</v>
+        <v>83</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>pashol na xuy</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,37 +2220,37 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>97</v>
+        <v>327</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>86</v>
+        <v>341</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>onangni sikay</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>11</v>
+        <v>184</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2259,24 +2259,24 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>92</v>
+        <v>363</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>oʻl</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2285,24 +2285,24 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>28</v>
+        <v>333</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>pashol na xuy</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2311,11 +2311,11 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>234</v>
+        <v>74</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,11 +2324,11 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2337,11 +2337,11 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>282</v>
+        <v>86</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2350,11 +2350,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,24 +2389,24 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>322</v>
+        <v>28</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>134</v>
+        <v>234</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,37 +2493,37 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>159</v>
+        <v>348</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>sexy woman</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>106</v>
+        <v>322</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,11 +2532,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2545,11 +2545,11 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2558,11 +2558,11 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2571,11 +2571,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>162</v>
+        <v>17</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>163</v>
+        <v>73</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,11 +2610,11 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2623,11 +2623,11 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2636,11 +2636,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,11 +2649,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2675,11 +2675,11 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>281</v>
+        <v>32</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2688,11 +2688,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2701,11 +2701,11 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>287</v>
+        <v>163</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2714,11 +2714,11 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2727,11 +2727,11 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2740,11 +2740,11 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2753,11 +2753,11 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2766,11 +2766,11 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2779,11 +2779,11 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>277</v>
+        <v>19</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2792,14 +2792,144 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
+        <v>281</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>yeban</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="n">
+        <v>148</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>yebanashka</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="n">
+        <v>287</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>yebat</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="n">
+        <v>91</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>yebbat</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="n">
+        <v>364</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>yeblan</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="n">
+        <v>145</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>yebnu</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="n">
+        <v>144</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>yebu</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="n">
+        <v>14</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="n">
+        <v>94</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="n">
+        <v>277</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="n">
         <v>283</v>
       </c>
-      <c r="B182" t="inlineStr">
+      <c r="B192" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C182" t="n">
+      <c r="C192" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-10-16 00:51:14 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -764,50 +764,50 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>214</v>
+        <v>367</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Jalla</t>
+          <t>Jalap</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>345</v>
+        <v>214</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Jallab</t>
+          <t>Jalla</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>151</v>
+        <v>345</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jallap</t>
+          <t>Jallab</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Jinni</t>
+          <t>Jallap</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -816,11 +816,11 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>205</v>
+        <v>56</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jipiriq</t>
+          <t>Jinni</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -829,50 +829,50 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>323</v>
+        <v>205</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kispurush</t>
+          <t>Jipiriq</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ko't</t>
+          <t>Kispurush</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>195</v>
+        <v>326</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kot</t>
+          <t>Ko't</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Kotinga</t>
+          <t>Kot</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -881,11 +881,11 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Koʻt</t>
+          <t>Kotinga</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -894,11 +894,11 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>129</v>
+        <v>194</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lox</t>
+          <t>Koʻt</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -907,11 +907,11 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>190</v>
+        <v>129</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Manjalaqi</t>
+          <t>Lox</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -920,11 +920,11 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>271</v>
+        <v>190</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Maraz</t>
+          <t>Manjalaqi</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -933,11 +933,11 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>207</v>
+        <v>271</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Mol miyya</t>
+          <t>Maraz</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -946,11 +946,11 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Om</t>
+          <t>Mol miyya</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -959,24 +959,24 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>318</v>
+        <v>212</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Onangni sikay</t>
+          <t>Om</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Onenei ami</t>
+          <t>Onangni sikay</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -985,11 +985,11 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Opangni omiga ske</t>
+          <t>Onenei ami</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -998,24 +998,24 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>298</v>
+        <v>339</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Pasholak</t>
+          <t>Opangni omiga ske</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>5</v>
+        <v>298</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Pidaraz</t>
+          <t>Pasholak</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1024,11 +1024,11 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>295</v>
+        <v>5</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Pidr</t>
+          <t>Pidaraz</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1037,11 +1037,11 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>156</v>
+        <v>295</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Pipez</t>
+          <t>Pidr</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1050,11 +1050,11 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>213</v>
+        <v>156</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Pizdes</t>
+          <t>Pipez</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1063,11 +1063,11 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Poxuy</t>
+          <t>Pizdes</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1076,11 +1076,11 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Poxxuy</t>
+          <t>Poxuy</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1089,37 +1089,37 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>325</v>
+        <v>114</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Pzdc</t>
+          <t>Poxxuy</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>154</v>
+        <v>325</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Pzds</t>
+          <t>Pzdc</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Pzdss</t>
+          <t>Pzds</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1128,11 +1128,11 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>269</v>
+        <v>155</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Qanchiq</t>
+          <t>Pzdss</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1141,11 +1141,11 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Qanciq</t>
+          <t>Qanchiq</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1154,11 +1154,11 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>189</v>
+        <v>270</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Qanjiq</t>
+          <t>Qanciq</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1167,11 +1167,11 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Qetoq</t>
+          <t>Qanjiq</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1180,37 +1180,37 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>358</v>
+        <v>211</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Qo'taq</t>
+          <t>Qetoq</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>172</v>
+        <v>358</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Qotaqxor</t>
+          <t>Qo'taq</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>257</v>
+        <v>172</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Qoto</t>
+          <t>Qotaqxor</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1219,11 +1219,11 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>169</v>
+        <v>257</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Qotoq</t>
+          <t>Qoto</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1232,11 +1232,11 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Qotoqbosh</t>
+          <t>Qotoq</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1245,11 +1245,11 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>210</v>
+        <v>25</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Qo’toq</t>
+          <t>Qotoqbosh</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1258,37 +1258,37 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>351</v>
+        <v>210</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Seks</t>
+          <t>Qo’toq</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>302</v>
+        <v>351</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Sen qishloqlisan</t>
+          <t>Seks</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>216</v>
+        <v>302</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Sik</t>
+          <t>Sen qishloqlisan</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1297,11 +1297,11 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Sikaman</t>
+          <t>Sik</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1310,37 +1310,37 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>352</v>
+        <v>215</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Sikay</t>
+          <t>Sikaman</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>113</v>
+        <v>352</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Sikdim</t>
+          <t>Sikay</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Ske</t>
+          <t>Sikdim</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1349,11 +1349,11 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>297</v>
+        <v>153</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Suchka</t>
+          <t>Ske</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1362,11 +1362,11 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>4</v>
+        <v>297</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Suka</t>
+          <t>Suchka</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1375,11 +1375,11 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>218</v>
+        <v>4</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Tashoq</t>
+          <t>Suka</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1388,11 +1388,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Tashshoq</t>
+          <t>Tashoq</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1401,37 +1401,37 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>316</v>
+        <v>217</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Tashshoq sho'rva</t>
+          <t>Tashshoq</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>219</v>
+        <v>316</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Tashshoq sho’rva</t>
+          <t>Tashshoq sho'rva</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Tente</t>
+          <t>Tashshoq sho’rva</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1440,11 +1440,11 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Xaromi</t>
+          <t>Tente</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1453,11 +1453,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Ya yebal tebya</t>
+          <t>Xaromi</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1466,11 +1466,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>233</v>
+        <v>143</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Yban</t>
+          <t>Ya yebal tebya</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1479,11 +1479,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Ybat</t>
+          <t>Yban</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1492,11 +1492,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Yeban</t>
+          <t>Ybat</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1505,11 +1505,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Yebanutiy</t>
+          <t>Yeban</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1518,11 +1518,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Yiban</t>
+          <t>Yebanutiy</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>183</v>
+        <v>2</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Zaybal</t>
+          <t>Yiban</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1544,11 +1544,11 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>78</v>
+        <v>183</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ahmoq</t>
+          <t>Zaybal</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1557,11 +1557,11 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ahuel</t>
+          <t>ahmoq</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,11 +1570,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>22</v>
+        <v>142</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>am</t>
+          <t>ahuel</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1583,37 +1583,37 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>329</v>
+        <v>22</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>ambaliq</t>
+          <t>am</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>223</v>
+        <v>329</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>amcha</t>
+          <t>ambaliq</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>108</v>
+        <v>223</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>aminga</t>
+          <t>amcha</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,76 +1622,76 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>349</v>
+        <v>108</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>amingga ske</t>
+          <t>aminga</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>axmoq</t>
+          <t>amingga ske</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>50</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>236</v>
+        <v>360</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>basharenga qotogm</t>
+          <t>axmoq</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>330</v>
+        <v>236</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>bich</t>
+          <t>basharenga qotogm</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>93</v>
+        <v>330</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>bich</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1700,11 +1700,11 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,11 +1713,11 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>261</v>
+        <v>53</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1726,11 +1726,11 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1739,11 +1739,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>244</v>
+        <v>262</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,11 +1778,11 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1791,11 +1791,11 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>107</v>
+        <v>305</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>278</v>
+        <v>107</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>84</v>
+        <v>278</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,11 +1830,11 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,37 +1843,37 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>324</v>
+        <v>110</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>111</v>
+        <v>324</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,37 +1882,37 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>361</v>
+        <v>160</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>garang</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>167</v>
+        <v>361</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>garang</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1921,11 +1921,11 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1934,11 +1934,11 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,11 +1947,11 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,63 +1960,63 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>334</v>
+        <v>203</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>idi naxuy</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>iflos</t>
+          <t>idi naxuy</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>48</v>
+        <v>90</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>iflos</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,11 +2038,11 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>303</v>
+        <v>98</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2051,11 +2051,11 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>76</v>
+        <v>303</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2064,11 +2064,11 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>158</v>
+        <v>76</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2077,11 +2077,11 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,76 +2116,76 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>26</v>
+        <v>366</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>kashanda</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>310</v>
+        <v>33</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>199</v>
+        <v>293</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>83</v>
+        <v>306</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2194,11 +2194,11 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>23</v>
+        <v>199</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,50 +2220,50 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>327</v>
+        <v>23</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>341</v>
+        <v>96</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>onangni sikay</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>184</v>
+        <v>327</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>oʻl</t>
+          <t>onangni sikay</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2272,50 +2272,50 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>12</v>
+        <v>365</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>oneni ami</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>333</v>
+        <v>184</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>pashol na xuy</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>75</v>
+        <v>363</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>oʻl</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,24 +2324,24 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>97</v>
+        <v>333</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>pashol na xuy</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2350,11 +2350,11 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,11 +2389,11 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2402,11 +2402,11 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>234</v>
+        <v>85</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>282</v>
+        <v>116</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>31</v>
+        <v>234</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>13</v>
+        <v>282</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,37 +2493,37 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>348</v>
+        <v>31</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>sexy woman</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>322</v>
+        <v>71</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,37 +2532,37 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>134</v>
+        <v>348</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>sexy woman</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2571,11 +2571,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,11 +2610,11 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>159</v>
+        <v>17</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2623,11 +2623,11 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2636,11 +2636,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,11 +2649,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2675,11 +2675,11 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2688,11 +2688,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2701,11 +2701,11 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2714,11 +2714,11 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2727,11 +2727,11 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2740,11 +2740,11 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2753,11 +2753,11 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2766,11 +2766,11 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>141</v>
+        <v>27</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2779,11 +2779,11 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2792,11 +2792,11 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>281</v>
+        <v>139</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2805,11 +2805,11 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2818,11 +2818,11 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>287</v>
+        <v>19</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2831,11 +2831,11 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>91</v>
+        <v>281</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2844,24 +2844,24 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>364</v>
+        <v>148</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>yeblan</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C186" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>145</v>
+        <v>287</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>yebat</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2870,11 +2870,11 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>yebbat</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2883,24 +2883,24 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>14</v>
+        <v>364</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yeblan</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yebnu</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -2909,11 +2909,11 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>277</v>
+        <v>144</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yebu</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2922,14 +2922,53 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
+        <v>14</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="n">
+        <v>94</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="n">
+        <v>277</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="n">
         <v>283</v>
       </c>
-      <c r="B192" t="inlineStr">
+      <c r="B195" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C192" t="n">
+      <c r="C195" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-11-15 00:52:38 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1778,24 +1778,24 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>280</v>
+        <v>368</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>cho'choq</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>107</v>
+        <v>305</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,11 +1817,11 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>278</v>
+        <v>107</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1830,11 +1830,11 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>84</v>
+        <v>278</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,11 +1843,11 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1856,37 +1856,37 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>324</v>
+        <v>110</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>111</v>
+        <v>324</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1895,37 +1895,37 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>361</v>
+        <v>160</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>garang</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>167</v>
+        <v>361</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>garang</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1934,11 +1934,11 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,11 +1947,11 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>227</v>
+        <v>161</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,11 +1960,11 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -1973,63 +1973,63 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>334</v>
+        <v>203</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>idi naxuy</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>iflos</t>
+          <t>idi naxuy</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>48</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>331</v>
+        <v>357</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>iflos</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,11 +2038,11 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2051,11 +2051,11 @@
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>303</v>
+        <v>98</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2064,11 +2064,11 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>76</v>
+        <v>303</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2077,11 +2077,11 @@
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>158</v>
+        <v>76</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,37 +2116,37 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>366</v>
+        <v>89</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>kashanda</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>33</v>
+        <v>366</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>kashanda</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2155,50 +2155,50 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>310</v>
+        <v>26</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>199</v>
+        <v>306</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2207,11 +2207,11 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>83</v>
+        <v>199</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,11 +2220,11 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2233,11 +2233,11 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2246,115 +2246,115 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>327</v>
+        <v>96</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>onangni sikay</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>oneni ami</t>
+          <t>onangni sikay</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>184</v>
+        <v>365</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>oneni ami</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>363</v>
+        <v>184</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>oʻl</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>12</v>
+        <v>363</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>oʻl</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>333</v>
+        <v>12</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>pashol na xuy</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>75</v>
+        <v>333</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>pashol na xuy</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2363,11 +2363,11 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,11 +2376,11 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,11 +2389,11 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2402,11 +2402,11 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2415,11 +2415,11 @@
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>116</v>
+        <v>28</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>234</v>
+        <v>116</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>72</v>
+        <v>234</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>282</v>
+        <v>72</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,11 +2493,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>31</v>
+        <v>282</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2506,11 +2506,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2519,11 +2519,11 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,50 +2532,50 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>348</v>
+        <v>13</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>sexy woman</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>sexy woman</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>109</v>
+        <v>322</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,11 +2610,11 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2623,11 +2623,11 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2636,11 +2636,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,11 +2649,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2675,11 +2675,11 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2688,11 +2688,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2701,11 +2701,11 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2714,11 +2714,11 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2727,11 +2727,11 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>162</v>
+        <v>32</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2740,11 +2740,11 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2753,11 +2753,11 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2766,11 +2766,11 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>27</v>
+        <v>137</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2779,11 +2779,11 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>140</v>
+        <v>27</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2792,11 +2792,11 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2805,11 +2805,11 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2818,11 +2818,11 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2831,11 +2831,11 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>281</v>
+        <v>19</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2844,11 +2844,11 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>148</v>
+        <v>281</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -2857,11 +2857,11 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>287</v>
+        <v>148</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2870,11 +2870,11 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>91</v>
+        <v>287</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>yebat</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2883,37 +2883,37 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>364</v>
+        <v>91</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>yeblan</t>
+          <t>yebbat</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>145</v>
+        <v>364</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>yeblan</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>yebnu</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2922,11 +2922,11 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>14</v>
+        <v>144</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yebu</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2935,11 +2935,11 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yetim</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2948,11 +2948,11 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>277</v>
+        <v>94</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yetm</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2961,14 +2961,27 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
+        <v>277</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="n">
         <v>283</v>
       </c>
-      <c r="B195" t="inlineStr">
+      <c r="B196" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C195" t="n">
+      <c r="C196" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2025-11-18 00:53:24 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1349,24 +1349,24 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>153</v>
+        <v>371</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ske</t>
+          <t>Skay</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>297</v>
+        <v>153</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Suchka</t>
+          <t>Ske</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1375,11 +1375,11 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>4</v>
+        <v>297</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Suka</t>
+          <t>Suchka</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1388,11 +1388,11 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>218</v>
+        <v>4</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Tashoq</t>
+          <t>Suka</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1401,11 +1401,11 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Tashshoq</t>
+          <t>Tashoq</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1414,37 +1414,37 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>316</v>
+        <v>217</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Tashshoq sho'rva</t>
+          <t>Tashshoq</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>68</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>219</v>
+        <v>316</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Tashshoq sho’rva</t>
+          <t>Tashshoq sho'rva</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>176</v>
+        <v>219</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Tente</t>
+          <t>Tashshoq sho’rva</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1453,11 +1453,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Xaromi</t>
+          <t>Tente</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1466,11 +1466,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>143</v>
+        <v>64</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Ya yebal tebya</t>
+          <t>Xaromi</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1479,11 +1479,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>233</v>
+        <v>143</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Yban</t>
+          <t>Ya yebal tebya</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1492,11 +1492,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Ybat</t>
+          <t>Yban</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1505,11 +1505,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Yeban</t>
+          <t>Ybat</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1518,11 +1518,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Yebanutiy</t>
+          <t>Yeban</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Yiban</t>
+          <t>Yebanutiy</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1544,24 +1544,24 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>183</v>
+        <v>373</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Zaybal</t>
+          <t>Yebat</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ahmoq</t>
+          <t>Yiban</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1570,24 +1570,24 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>142</v>
+        <v>372</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ahuel</t>
+          <t>Yobbana</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>am</t>
+          <t>Zaybal</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1596,24 +1596,24 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>329</v>
+        <v>78</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>ambaliq</t>
+          <t>ahmoq</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>223</v>
+        <v>142</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>amcha</t>
+          <t>ahuel</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1622,11 +1622,11 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>108</v>
+        <v>22</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>aminga</t>
+          <t>am</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1635,37 +1635,37 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>amingga ske</t>
+          <t>ambaliq</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>97</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>360</v>
+        <v>223</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>axmoq</t>
+          <t>amcha</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>236</v>
+        <v>108</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>basharenga qotogm</t>
+          <t>aminga</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1674,37 +1674,37 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>330</v>
+        <v>349</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>bich</t>
+          <t>amingga ske</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>50</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>93</v>
+        <v>360</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>bitch</t>
+          <t>axmoq</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>99</v>
+        <v>236</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>ble</t>
+          <t>basharenga qotogm</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1713,24 +1713,24 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>53</v>
+        <v>330</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>blet</t>
+          <t>bich</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>261</v>
+        <v>93</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>bo'qidish</t>
+          <t>bitch</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1739,11 +1739,11 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>262</v>
+        <v>99</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>bo'qkalla</t>
+          <t>ble</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1752,11 +1752,11 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>244</v>
+        <v>53</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>boq</t>
+          <t>blet</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1765,11 +1765,11 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>bo'qidish</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1778,24 +1778,24 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>368</v>
+        <v>262</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>cho'choq</t>
+          <t>bo'qkalla</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>boq</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1804,11 +1804,11 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1817,24 +1817,24 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>107</v>
+        <v>368</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>cho'choq</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,11 +1843,11 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>84</v>
+        <v>305</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1856,37 +1856,37 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>110</v>
+        <v>370</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>dalban</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>324</v>
+        <v>107</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>111</v>
+        <v>278</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1895,11 +1895,11 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>160</v>
+        <v>84</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1908,37 +1908,37 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>361</v>
+        <v>110</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>garang</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>167</v>
+        <v>324</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>166</v>
+        <v>111</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1947,11 +1947,11 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,24 +1960,24 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>227</v>
+        <v>361</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>garang</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1986,50 +1986,50 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>334</v>
+        <v>166</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>idi naxuy</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>357</v>
+        <v>161</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>iflos</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>331</v>
+        <v>227</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>260</v>
+        <v>203</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,50 +2038,50 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>95</v>
+        <v>334</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>idi naxuy</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>98</v>
+        <v>357</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>iflos</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>76</v>
+        <v>260</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2090,11 +2090,11 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2103,11 +2103,11 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2116,11 +2116,11 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>89</v>
+        <v>303</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,24 +2129,24 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>366</v>
+        <v>76</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>kashanda</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2155,11 +2155,11 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,50 +2168,50 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>310</v>
+        <v>89</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>293</v>
+        <v>374</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>jentra miyya</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>306</v>
+        <v>366</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>kashanda</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>199</v>
+        <v>33</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,11 +2220,11 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2233,76 +2233,76 @@
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>23</v>
+        <v>310</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>96</v>
+        <v>293</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>341</v>
+        <v>199</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>onangni sikay</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>365</v>
+        <v>83</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>oneni ami</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>184</v>
+        <v>23</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2311,63 +2311,63 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>363</v>
+        <v>96</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>oʻl</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>12</v>
+        <v>327</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>pashol na xuy</t>
+          <t>onangni sikay</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>75</v>
+        <v>365</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>oneni ami</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>74</v>
+        <v>184</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2376,24 +2376,24 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>97</v>
+        <v>363</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>oʻl</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2402,24 +2402,24 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>11</v>
+        <v>333</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>pashol na xuy</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2428,11 +2428,11 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,11 +2441,11 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2454,11 +2454,11 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>234</v>
+        <v>11</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,11 +2493,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>282</v>
+        <v>85</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2506,11 +2506,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2519,11 +2519,11 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,11 +2532,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>13</v>
+        <v>234</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2545,37 +2545,37 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>348</v>
+        <v>72</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>sexy woman</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C163" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>322</v>
+        <v>282</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,37 +2610,37 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>20</v>
+        <v>348</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>sexy woman</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>17</v>
+        <v>322</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,11 +2649,11 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2662,11 +2662,11 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>159</v>
+        <v>18</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2675,11 +2675,11 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2688,11 +2688,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2701,11 +2701,11 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>119</v>
+        <v>73</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2714,11 +2714,11 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2727,11 +2727,11 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>32</v>
+        <v>159</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2740,11 +2740,11 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2753,11 +2753,11 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2766,11 +2766,11 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2779,11 +2779,11 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2792,11 +2792,11 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>140</v>
+        <v>32</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2805,11 +2805,11 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2818,11 +2818,11 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2831,11 +2831,11 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2844,11 +2844,11 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>281</v>
+        <v>27</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -2857,11 +2857,11 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2870,11 +2870,11 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>287</v>
+        <v>139</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2883,11 +2883,11 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -2896,24 +2896,24 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>364</v>
+        <v>19</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>yeblan</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>145</v>
+        <v>281</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2922,11 +2922,11 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2935,11 +2935,11 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>14</v>
+        <v>287</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yebat</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2948,11 +2948,11 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yebbat</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2961,27 +2961,92 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>277</v>
+        <v>364</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yeblan</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
+        <v>145</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>yebnu</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="n">
+        <v>144</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>yebu</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="n">
+        <v>14</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="n">
+        <v>94</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="n">
+        <v>277</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="n">
         <v>283</v>
       </c>
-      <c r="B196" t="inlineStr">
+      <c r="B201" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C196" t="n">
+      <c r="C201" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto‑update: 2026-01-26 01:03:52 UTC
</commit_message>
<xml_diff>
--- a/resources/bad_words.xlsx
+++ b/resources/bad_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:C204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1804,37 +1804,37 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>279</v>
+        <v>9</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>chmo</t>
+          <t>buvini ami</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>368</v>
+        <v>10</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>cho'choq</t>
+          <t>buvini amiga ske</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>chumo</t>
+          <t>chmo</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1843,37 +1843,37 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>305</v>
+        <v>368</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>dabba</t>
+          <t>cho'choq</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>370</v>
+        <v>280</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>dalban</t>
+          <t>chumo</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>107</v>
+        <v>305</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>dalbayob</t>
+          <t>dabba</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1882,24 +1882,24 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>278</v>
+        <v>370</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>daun</t>
+          <t>dalban</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>dinnaxuy</t>
+          <t>dalbayob</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1908,11 +1908,11 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>fuck</t>
+          <t>daun</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1921,37 +1921,37 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>324</v>
+        <v>84</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>fuck off</t>
+          <t>dinnaxuy</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>111</v>
+        <v>8</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>fucking</t>
+          <t>foxisha qanchiq</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>gandon</t>
+          <t>fuck</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1960,24 +1960,24 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>garang</t>
+          <t>fuck off</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>gay</t>
+          <t>fucking</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1986,11 +1986,11 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>gey</t>
+          <t>gandon</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -1999,24 +1999,24 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>161</v>
+        <v>361</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>gnida</t>
+          <t>garang</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>227</v>
+        <v>167</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>haromi</t>
+          <t>gay</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2025,11 +2025,11 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>hunasa</t>
+          <t>gey</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2038,89 +2038,89 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>334</v>
+        <v>161</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>idi naxuy</t>
+          <t>gnida</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>357</v>
+        <v>227</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>iflos</t>
+          <t>haromi</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>331</v>
+        <v>203</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>it</t>
+          <t>hunasa</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>260</v>
+        <v>334</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>itbet</t>
+          <t>idi naxuy</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>95</v>
+        <v>357</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>jala</t>
+          <t>iflos</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>98</v>
+        <v>331</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>jala ble</t>
+          <t>it</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>303</v>
+        <v>260</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>jalaaap</t>
+          <t>itbet</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2129,11 +2129,11 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>jalab</t>
+          <t>jala</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2142,11 +2142,11 @@
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>jalap</t>
+          <t>jala ble</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2155,11 +2155,11 @@
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>88</v>
+        <v>303</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>jalla</t>
+          <t>jalaaap</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2168,11 +2168,11 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>jallap</t>
+          <t>jalab</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2181,37 +2181,37 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>374</v>
+        <v>158</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>jentra miyya</t>
+          <t>jalap</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>366</v>
+        <v>88</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>kashanda</t>
+          <t>jalla</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>ko't</t>
+          <t>jallap</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2220,50 +2220,50 @@
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>26</v>
+        <v>374</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>kot</t>
+          <t>jentra miyya</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>310</v>
+        <v>366</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>lox</t>
+          <t>kashanda</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>293</v>
+        <v>33</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>mol</t>
+          <t>ko't</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>306</v>
+        <v>26</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>nedagon</t>
+          <t>kot</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2272,37 +2272,37 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>199</v>
+        <v>310</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>nigga</t>
+          <t>lox</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>83</v>
+        <v>293</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>nigger</t>
+          <t>mol</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>23</v>
+        <v>306</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>nedagon</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2311,11 +2311,11 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>96</v>
+        <v>199</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>onangni</t>
+          <t>nigga</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2324,63 +2324,63 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>327</v>
+        <v>83</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>onangni ami</t>
+          <t>nigger</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>341</v>
+        <v>23</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>onangni sikay</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>365</v>
+        <v>96</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>oneni ami</t>
+          <t>onangni</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>184</v>
+        <v>327</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>oom</t>
+          <t>onangni ami</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>oʻl</t>
+          <t>onangni sikay</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2389,50 +2389,50 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>12</v>
+        <v>365</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>p1zdes</t>
+          <t>oneni ami</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>333</v>
+        <v>184</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>pashol na xuy</t>
+          <t>oom</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>75</v>
+        <v>363</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>pidaras</t>
+          <t>oʻl</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>pidaraz</t>
+          <t>p1zdes</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2441,24 +2441,24 @@
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>97</v>
+        <v>333</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>pidr</t>
+          <t>pashol na xuy</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>pizda</t>
+          <t>pidaras</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2467,11 +2467,11 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>pizdes</t>
+          <t>pidaraz</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2480,11 +2480,11 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>qanjiq</t>
+          <t>pidr</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2493,11 +2493,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>qo'toq</t>
+          <t>pizda</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2506,11 +2506,11 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>qo'toqbosh</t>
+          <t>pizdes</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2519,11 +2519,11 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>qotaq</t>
+          <t>qanjiq</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2532,11 +2532,11 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>234</v>
+        <v>85</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>qoto</t>
+          <t>qo'toq</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2545,11 +2545,11 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>qotoq</t>
+          <t>qo'toqbosh</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2558,11 +2558,11 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>282</v>
+        <v>116</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>qutoq</t>
+          <t>qotaq</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2571,11 +2571,11 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>31</v>
+        <v>234</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>seks</t>
+          <t>qoto</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2584,11 +2584,11 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>seksi baby</t>
+          <t>qotoq</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>13</v>
+        <v>282</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>qutoq</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2610,37 +2610,37 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>348</v>
+        <v>31</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>sexy woman</t>
+          <t>seks</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>322</v>
+        <v>71</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>shavqatsiz</t>
+          <t>seksi baby</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>sikay</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2649,37 +2649,37 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>134</v>
+        <v>348</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>sike</t>
+          <t>sexy woman</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>18</v>
+        <v>322</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>sikish</t>
+          <t>shavqatsiz</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>siktim</t>
+          <t>sikay</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2688,11 +2688,11 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>sikvoti</t>
+          <t>sike</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2701,11 +2701,11 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>skay</t>
+          <t>sikish</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2714,11 +2714,11 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>ske</t>
+          <t>siktim</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2727,11 +2727,11 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>159</v>
+        <v>17</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>skey</t>
+          <t>sikvoti</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2740,11 +2740,11 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>suchka</t>
+          <t>skay</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2753,11 +2753,11 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>suka</t>
+          <t>ske</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2766,11 +2766,11 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>sukka</t>
+          <t>skey</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2779,11 +2779,11 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>tashsho</t>
+          <t>suchka</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2792,11 +2792,11 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>tupoy</t>
+          <t>suka</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2805,11 +2805,11 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>tvar</t>
+          <t>sukka</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2818,11 +2818,11 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>163</v>
+        <v>87</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>tvariddin</t>
+          <t>tashsho</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2831,11 +2831,11 @@
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>wtf</t>
+          <t>tupoy</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2844,11 +2844,11 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>xaromi</t>
+          <t>tvar</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -2857,11 +2857,11 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>xuyeplet</t>
+          <t>tvariddin</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2870,11 +2870,11 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>xuyesos</t>
+          <t>wtf</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2883,11 +2883,11 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>141</v>
+        <v>27</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>xuyila</t>
+          <t>xaromi</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -2896,11 +2896,11 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>yban</t>
+          <t>xuyeplet</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -2909,11 +2909,11 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>281</v>
+        <v>139</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>yeban</t>
+          <t>xuyesos</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2922,11 +2922,11 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>yebanashka</t>
+          <t>xuyila</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2935,11 +2935,11 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>287</v>
+        <v>19</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>yebat</t>
+          <t>yban</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2948,11 +2948,11 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>91</v>
+        <v>281</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>yebbat</t>
+          <t>yeban</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2961,24 +2961,24 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>364</v>
+        <v>148</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>yeblan</t>
+          <t>yebanashka</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>145</v>
+        <v>287</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>yebnu</t>
+          <t>yebat</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -2987,11 +2987,11 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>yebu</t>
+          <t>yebbat</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -3000,24 +3000,24 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>14</v>
+        <v>364</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>yetim</t>
+          <t>yeblan</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>yetm</t>
+          <t>yebnu</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -3026,11 +3026,11 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>277</v>
+        <v>144</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>yiban</t>
+          <t>yebu</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -3039,14 +3039,53 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
+        <v>14</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>yetim</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>94</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>yetm</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>277</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>yiban</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
         <v>283</v>
       </c>
-      <c r="B201" t="inlineStr">
+      <c r="B204" t="inlineStr">
         <is>
           <t>yibanat</t>
         </is>
       </c>
-      <c r="C201" t="n">
+      <c r="C204" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>